<commit_message>
New prompt format with order
</commit_message>
<xml_diff>
--- a/resources/keyword_dict_annotated.xlsx
+++ b/resources/keyword_dict_annotated.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="911" uniqueCount="545">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="546">
   <si>
     <t>class</t>
   </si>
@@ -107,6 +107,9 @@
   </si>
   <si>
     <t>['roused him from his kip']</t>
+  </si>
+  <si>
+    <t>dozing</t>
   </si>
   <si>
     <t>death</t>
@@ -1713,7 +1716,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1725,6 +1728,9 @@
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -2035,17 +2041,17 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E234"/>
+  <dimension ref="A1:E235"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="22.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="85.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="22.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="85.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
@@ -2257,7 +2263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="3" t="s">
         <v>8</v>
       </c>
@@ -2265,13 +2271,11 @@
         <v>31</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E14" s="4">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="5">
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
@@ -2279,16 +2283,16 @@
         <v>8</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="E15" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
@@ -2296,13 +2300,13 @@
         <v>8</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>37</v>
-      </c>
       <c r="D16" s="3" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="E16" s="4">
         <v>1</v>
@@ -2313,13 +2317,13 @@
         <v>8</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="E17" s="4">
         <v>1</v>
@@ -2330,13 +2334,13 @@
         <v>8</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>44</v>
       </c>
       <c r="E18" s="4">
         <v>1</v>
@@ -2347,61 +2351,61 @@
         <v>8</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>47</v>
-      </c>
       <c r="E19" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+        <v>1</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B20" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="E20" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+      <c r="A21" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="C21" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E20" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
-      <c r="A21" s="3" t="s">
+      <c r="D21" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="E21" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B22" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>55</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>15</v>
@@ -2412,64 +2416,64 @@
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B23" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="D23" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
+      <c r="A24" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E23" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
-      <c r="A24" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B24" s="3" t="s">
+      <c r="C24" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>59</v>
-      </c>
       <c r="D24" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E24" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B25" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>61</v>
-      </c>
       <c r="D25" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E25" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B26" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>63</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>15</v>
@@ -2480,13 +2484,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
       <c r="A27" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>65</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>15</v>
@@ -2497,13 +2501,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
       <c r="A28" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B28" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>15</v>
@@ -2514,13 +2518,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
       <c r="A29" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B29" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>69</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>15</v>
@@ -2531,13 +2535,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
       <c r="A30" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B30" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>71</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>15</v>
@@ -2548,13 +2552,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
       <c r="A31" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B31" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>72</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>73</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>15</v>
@@ -2565,13 +2569,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
       <c r="A32" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B32" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>75</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>15</v>
@@ -2582,13 +2586,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
       <c r="A33" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B33" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>76</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>77</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>15</v>
@@ -2599,13 +2603,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
       <c r="A34" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B34" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>78</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>79</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>15</v>
@@ -2616,13 +2620,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
       <c r="A35" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B35" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>81</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>15</v>
@@ -2633,13 +2637,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
       <c r="A36" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B36" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C36" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>83</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>15</v>
@@ -2650,16 +2654,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
       <c r="A37" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B37" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C37" s="3" t="s">
-        <v>85</v>
-      </c>
       <c r="D37" s="3" t="s">
-        <v>86</v>
+        <v>15</v>
       </c>
       <c r="E37" s="4">
         <v>1</v>
@@ -2667,16 +2671,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
       <c r="A38" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B38" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D38" s="3" t="s">
         <v>87</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>89</v>
       </c>
       <c r="E38" s="4">
         <v>1</v>
@@ -2684,16 +2688,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
       <c r="A39" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B39" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D39" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>92</v>
       </c>
       <c r="E39" s="4">
         <v>1</v>
@@ -2701,16 +2705,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
       <c r="A40" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B40" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D40" s="3" t="s">
         <v>93</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>95</v>
       </c>
       <c r="E40" s="4">
         <v>1</v>
@@ -2718,67 +2722,67 @@
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
       <c r="A41" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B41" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D41" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C41" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>98</v>
-      </c>
       <c r="E41" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
       <c r="A42" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B42" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D42" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C42" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>101</v>
-      </c>
       <c r="E42" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
       <c r="A43" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B43" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D43" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C43" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="E43" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
       <c r="A44" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B44" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C44" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="C44" s="3" t="s">
-        <v>105</v>
-      </c>
       <c r="D44" s="3" t="s">
-        <v>106</v>
+        <v>15</v>
       </c>
       <c r="E44" s="4">
         <v>0</v>
@@ -2786,16 +2790,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
       <c r="A45" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B45" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D45" s="3" t="s">
         <v>107</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>109</v>
       </c>
       <c r="E45" s="4">
         <v>0</v>
@@ -2803,33 +2807,33 @@
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
       <c r="A46" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B46" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D46" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="C46" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="E46" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
       <c r="A47" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B47" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C47" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="C47" s="3" t="s">
-        <v>113</v>
-      </c>
       <c r="D47" s="3" t="s">
-        <v>114</v>
+        <v>15</v>
       </c>
       <c r="E47" s="4">
         <v>1</v>
@@ -2837,16 +2841,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
       <c r="A48" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B48" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D48" s="3" t="s">
         <v>115</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>117</v>
       </c>
       <c r="E48" s="4">
         <v>1</v>
@@ -2854,16 +2858,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
       <c r="A49" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B49" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D49" s="3" t="s">
         <v>118</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="E49" s="4">
         <v>1</v>
@@ -2871,33 +2875,33 @@
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
       <c r="A50" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B50" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C50" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="C50" s="3" t="s">
-        <v>121</v>
-      </c>
       <c r="D50" s="3" t="s">
-        <v>122</v>
+        <v>15</v>
       </c>
       <c r="E50" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
       <c r="A51" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B51" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D51" s="3" t="s">
         <v>123</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>125</v>
       </c>
       <c r="E51" s="4">
         <v>0</v>
@@ -2905,33 +2909,33 @@
     </row>
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
       <c r="A52" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B52" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D52" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="C52" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>128</v>
-      </c>
       <c r="E52" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
       <c r="A53" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B53" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D53" s="3" t="s">
         <v>129</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>131</v>
       </c>
       <c r="E53" s="4">
         <v>1</v>
@@ -2939,33 +2943,33 @@
     </row>
     <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
       <c r="A54" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B54" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="D54" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="C54" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>134</v>
-      </c>
       <c r="E54" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
       <c r="A55" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B55" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D55" s="3" t="s">
         <v>135</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>137</v>
       </c>
       <c r="E55" s="4">
         <v>0</v>
@@ -2973,33 +2977,33 @@
     </row>
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
       <c r="A56" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B56" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D56" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C56" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>140</v>
-      </c>
       <c r="E56" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
       <c r="A57" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B57" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D57" s="3" t="s">
         <v>141</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>143</v>
       </c>
       <c r="E57" s="4">
         <v>1</v>
@@ -3007,16 +3011,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
       <c r="A58" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B58" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D58" s="3" t="s">
         <v>144</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>146</v>
       </c>
       <c r="E58" s="4">
         <v>1</v>
@@ -3024,16 +3028,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
       <c r="A59" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B59" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D59" s="3" t="s">
         <v>147</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>149</v>
       </c>
       <c r="E59" s="4">
         <v>1</v>
@@ -3041,16 +3045,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
       <c r="A60" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B60" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D60" s="3" t="s">
         <v>150</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="E60" s="4">
         <v>1</v>
@@ -3058,13 +3062,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
       <c r="A61" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B61" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C61" s="3" t="s">
         <v>152</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>153</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>15</v>
@@ -3075,13 +3079,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75">
       <c r="A62" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B62" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C62" s="3" t="s">
         <v>154</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>155</v>
       </c>
       <c r="D62" s="3" t="s">
         <v>15</v>
@@ -3092,16 +3096,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75">
       <c r="A63" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B63" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C63" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="C63" s="3" t="s">
-        <v>157</v>
-      </c>
       <c r="D63" s="3" t="s">
-        <v>158</v>
+        <v>15</v>
       </c>
       <c r="E63" s="4">
         <v>1</v>
@@ -3109,16 +3113,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18.75">
       <c r="A64" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B64" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D64" s="3" t="s">
         <v>159</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>161</v>
       </c>
       <c r="E64" s="4">
         <v>1</v>
@@ -3126,135 +3130,135 @@
     </row>
     <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75">
       <c r="A65" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B65" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D65" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="C65" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="E65" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75">
       <c r="A66" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B66" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C66" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="C66" s="3" t="s">
-        <v>165</v>
-      </c>
       <c r="D66" s="3" t="s">
-        <v>166</v>
+        <v>15</v>
       </c>
       <c r="E66" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75">
       <c r="A67" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B67" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="D67" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="C67" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="D67" s="3" t="s">
-        <v>169</v>
-      </c>
       <c r="E67" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75">
       <c r="A68" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B68" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="D68" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="C68" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="D68" s="3" t="s">
-        <v>172</v>
-      </c>
       <c r="E68" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75">
       <c r="A69" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B69" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D69" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="C69" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="D69" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="E69" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75">
       <c r="A70" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B70" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C70" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="C70" s="3" t="s">
-        <v>176</v>
-      </c>
       <c r="D70" s="3" t="s">
-        <v>177</v>
+        <v>15</v>
       </c>
       <c r="E70" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18.75">
       <c r="A71" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B71" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="D71" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="C71" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>180</v>
-      </c>
       <c r="E71" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18.75">
       <c r="A72" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B72" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="D72" s="3" t="s">
         <v>181</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="D72" s="3" t="s">
-        <v>183</v>
       </c>
       <c r="E72" s="4">
         <v>0</v>
@@ -3262,16 +3266,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75">
       <c r="A73" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B73" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="D73" s="3" t="s">
         <v>184</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="D73" s="3" t="s">
-        <v>186</v>
       </c>
       <c r="E73" s="4">
         <v>0</v>
@@ -3279,50 +3283,50 @@
     </row>
     <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18.75">
       <c r="A74" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B74" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D74" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="C74" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="D74" s="3" t="s">
-        <v>189</v>
-      </c>
       <c r="E74" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18.75">
       <c r="A75" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B75" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="D75" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="C75" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="D75" s="3" t="s">
-        <v>192</v>
-      </c>
       <c r="E75" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18.75">
       <c r="A76" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B76" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="D76" s="3" t="s">
         <v>193</v>
-      </c>
-      <c r="C76" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="D76" s="3" t="s">
-        <v>195</v>
       </c>
       <c r="E76" s="4">
         <v>0</v>
@@ -3330,16 +3334,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75">
       <c r="A77" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B77" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="D77" s="3" t="s">
         <v>196</v>
-      </c>
-      <c r="C77" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="D77" s="3" t="s">
-        <v>198</v>
       </c>
       <c r="E77" s="4">
         <v>0</v>
@@ -3347,16 +3351,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75">
       <c r="A78" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B78" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D78" s="3" t="s">
         <v>199</v>
-      </c>
-      <c r="C78" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="D78" s="3" t="s">
-        <v>201</v>
       </c>
       <c r="E78" s="4">
         <v>0</v>
@@ -3364,16 +3368,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75">
       <c r="A79" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B79" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D79" s="3" t="s">
         <v>202</v>
-      </c>
-      <c r="C79" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="D79" s="3" t="s">
-        <v>204</v>
       </c>
       <c r="E79" s="4">
         <v>0</v>
@@ -3381,16 +3385,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18.75">
       <c r="A80" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B80" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="D80" s="3" t="s">
         <v>205</v>
-      </c>
-      <c r="C80" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="D80" s="3" t="s">
-        <v>207</v>
       </c>
       <c r="E80" s="4">
         <v>0</v>
@@ -3398,16 +3402,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18.75">
       <c r="A81" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B81" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="D81" s="3" t="s">
         <v>208</v>
-      </c>
-      <c r="C81" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="D81" s="3" t="s">
-        <v>210</v>
       </c>
       <c r="E81" s="4">
         <v>0</v>
@@ -3415,16 +3419,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18.75">
       <c r="A82" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B82" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="D82" s="3" t="s">
         <v>211</v>
-      </c>
-      <c r="C82" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="D82" s="3" t="s">
-        <v>213</v>
       </c>
       <c r="E82" s="4">
         <v>0</v>
@@ -3432,16 +3436,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18.75">
       <c r="A83" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B83" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="D83" s="3" t="s">
         <v>214</v>
-      </c>
-      <c r="C83" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="D83" s="3" t="s">
-        <v>216</v>
       </c>
       <c r="E83" s="4">
         <v>0</v>
@@ -3449,64 +3453,64 @@
     </row>
     <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="18.75">
       <c r="A84" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="D84" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="B84" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="C84" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="D84" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="E84" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18.75">
       <c r="A85" s="3" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B85" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C85" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="C85" s="3" t="s">
-        <v>221</v>
-      </c>
       <c r="D85" s="3" t="s">
-        <v>222</v>
+        <v>15</v>
       </c>
       <c r="E85" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18.75">
       <c r="A86" s="3" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B86" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="D86" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="C86" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="D86" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="E86" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18.75">
       <c r="A87" s="3" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B87" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="C87" s="3" t="s">
         <v>225</v>
-      </c>
-      <c r="C87" s="3" t="s">
-        <v>226</v>
       </c>
       <c r="D87" s="3" t="s">
         <v>15</v>
@@ -3517,13 +3521,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18.75">
       <c r="A88" s="3" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B88" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="C88" s="3" t="s">
         <v>227</v>
-      </c>
-      <c r="C88" s="3" t="s">
-        <v>228</v>
       </c>
       <c r="D88" s="3" t="s">
         <v>15</v>
@@ -3534,13 +3538,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18.75">
       <c r="A89" s="3" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B89" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="C89" s="3" t="s">
         <v>229</v>
-      </c>
-      <c r="C89" s="3" t="s">
-        <v>230</v>
       </c>
       <c r="D89" s="3" t="s">
         <v>15</v>
@@ -3551,16 +3555,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18.75">
       <c r="A90" s="3" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B90" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="C90" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="C90" s="3" t="s">
-        <v>232</v>
-      </c>
       <c r="D90" s="3" t="s">
-        <v>233</v>
+        <v>15</v>
       </c>
       <c r="E90" s="4">
         <v>1</v>
@@ -3568,16 +3572,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18.75">
       <c r="A91" s="3" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B91" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="D91" s="3" t="s">
         <v>234</v>
-      </c>
-      <c r="C91" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="D91" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="E91" s="4">
         <v>1</v>
@@ -3585,13 +3589,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="18.75">
       <c r="A92" s="3" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B92" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="C92" s="3" t="s">
         <v>236</v>
-      </c>
-      <c r="C92" s="3" t="s">
-        <v>237</v>
       </c>
       <c r="D92" s="3" t="s">
         <v>15</v>
@@ -3602,13 +3606,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18.75">
       <c r="A93" s="3" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B93" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="C93" s="3" t="s">
         <v>238</v>
-      </c>
-      <c r="C93" s="3" t="s">
-        <v>239</v>
       </c>
       <c r="D93" s="3" t="s">
         <v>15</v>
@@ -3619,13 +3623,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="18.75">
       <c r="A94" s="3" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B94" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="C94" s="3" t="s">
         <v>240</v>
-      </c>
-      <c r="C94" s="3" t="s">
-        <v>241</v>
       </c>
       <c r="D94" s="3" t="s">
         <v>15</v>
@@ -3636,16 +3640,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="18.75">
       <c r="A95" s="3" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B95" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="C95" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="C95" s="3" t="s">
-        <v>243</v>
-      </c>
       <c r="D95" s="3" t="s">
-        <v>244</v>
+        <v>15</v>
       </c>
       <c r="E95" s="4">
         <v>1</v>
@@ -3653,30 +3657,30 @@
     </row>
     <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18.75">
       <c r="A96" s="3" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B96" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="D96" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="C96" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="D96" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="E96" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18.75">
       <c r="A97" s="3" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B97" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="C97" s="3" t="s">
         <v>247</v>
-      </c>
-      <c r="C97" s="3" t="s">
-        <v>248</v>
       </c>
       <c r="D97" s="3" t="s">
         <v>15</v>
@@ -3687,77 +3691,77 @@
     </row>
     <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="18.75">
       <c r="A98" s="3" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B98" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C98" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="C98" s="3"/>
-      <c r="D98" s="3"/>
+      <c r="D98" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="E98" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="18.75">
       <c r="A99" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="B99" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="B99" s="3" t="s">
-        <v>251</v>
-      </c>
-      <c r="C99" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="D99" s="3" t="s">
-        <v>253</v>
-      </c>
+      <c r="C99" s="3"/>
+      <c r="D99" s="3"/>
       <c r="E99" s="4">
         <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="18.75">
       <c r="A100" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B100" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="C100" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="D100" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="C100" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="D100" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="E100" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="18.75">
       <c r="A101" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B101" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="C101" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="C101" s="3" t="s">
-        <v>257</v>
-      </c>
       <c r="D101" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E101" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="18.75">
       <c r="A102" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B102" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="C102" s="3" t="s">
         <v>258</v>
-      </c>
-      <c r="C102" s="3" t="s">
-        <v>259</v>
       </c>
       <c r="D102" s="3" t="s">
         <v>15</v>
@@ -3768,13 +3772,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="18.75">
       <c r="A103" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B103" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="C103" s="3" t="s">
         <v>260</v>
-      </c>
-      <c r="C103" s="3" t="s">
-        <v>261</v>
       </c>
       <c r="D103" s="3" t="s">
         <v>15</v>
@@ -3785,13 +3789,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="18.75">
       <c r="A104" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B104" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="C104" s="3" t="s">
         <v>262</v>
-      </c>
-      <c r="C104" s="3" t="s">
-        <v>263</v>
       </c>
       <c r="D104" s="3" t="s">
         <v>15</v>
@@ -3802,13 +3806,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="18.75">
       <c r="A105" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B105" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="C105" s="3" t="s">
         <v>264</v>
-      </c>
-      <c r="C105" s="3" t="s">
-        <v>265</v>
       </c>
       <c r="D105" s="3" t="s">
         <v>15</v>
@@ -3819,47 +3823,47 @@
     </row>
     <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="18.75">
       <c r="A106" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B106" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="C106" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="C106" s="3" t="s">
-        <v>267</v>
-      </c>
       <c r="D106" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E106" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="18.75">
       <c r="A107" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B107" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="C107" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="C107" s="3" t="s">
-        <v>269</v>
-      </c>
       <c r="D107" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E107" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="18.75">
       <c r="A108" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B108" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="C108" s="3" t="s">
         <v>270</v>
-      </c>
-      <c r="C108" s="3" t="s">
-        <v>271</v>
       </c>
       <c r="D108" s="3" t="s">
         <v>15</v>
@@ -3870,16 +3874,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="18.75">
       <c r="A109" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B109" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="C109" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="C109" s="3" t="s">
-        <v>273</v>
-      </c>
       <c r="D109" s="3" t="s">
-        <v>274</v>
+        <v>15</v>
       </c>
       <c r="E109" s="4">
         <v>1</v>
@@ -3887,16 +3891,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="18.75">
       <c r="A110" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B110" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="C110" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="D110" s="3" t="s">
         <v>275</v>
-      </c>
-      <c r="C110" s="3" t="s">
-        <v>276</v>
-      </c>
-      <c r="D110" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="E110" s="4">
         <v>1</v>
@@ -3904,13 +3908,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="18.75">
       <c r="A111" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B111" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="C111" s="3" t="s">
         <v>277</v>
-      </c>
-      <c r="C111" s="3" t="s">
-        <v>278</v>
       </c>
       <c r="D111" s="3" t="s">
         <v>15</v>
@@ -3921,13 +3925,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="18.75">
       <c r="A112" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B112" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="C112" s="3" t="s">
         <v>279</v>
-      </c>
-      <c r="C112" s="3" t="s">
-        <v>280</v>
       </c>
       <c r="D112" s="3" t="s">
         <v>15</v>
@@ -3938,13 +3942,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="18.75">
       <c r="A113" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B113" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="C113" s="3" t="s">
         <v>281</v>
-      </c>
-      <c r="C113" s="3" t="s">
-        <v>282</v>
       </c>
       <c r="D113" s="3" t="s">
         <v>15</v>
@@ -3955,13 +3959,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="18.75">
       <c r="A114" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B114" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="C114" s="3" t="s">
         <v>283</v>
-      </c>
-      <c r="C114" s="3" t="s">
-        <v>284</v>
       </c>
       <c r="D114" s="3" t="s">
         <v>15</v>
@@ -3972,13 +3976,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="18.75">
       <c r="A115" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B115" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="C115" s="3" t="s">
         <v>285</v>
-      </c>
-      <c r="C115" s="3" t="s">
-        <v>286</v>
       </c>
       <c r="D115" s="3" t="s">
         <v>15</v>
@@ -3989,13 +3993,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="18.75">
       <c r="A116" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B116" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="C116" s="3" t="s">
         <v>287</v>
-      </c>
-      <c r="C116" s="3" t="s">
-        <v>288</v>
       </c>
       <c r="D116" s="3" t="s">
         <v>15</v>
@@ -4006,13 +4010,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="117" customHeight="1" ht="18.75">
       <c r="A117" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B117" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="C117" s="3" t="s">
         <v>289</v>
-      </c>
-      <c r="C117" s="3" t="s">
-        <v>290</v>
       </c>
       <c r="D117" s="3" t="s">
         <v>15</v>
@@ -4023,13 +4027,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="118" customHeight="1" ht="18.75">
       <c r="A118" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B118" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="C118" s="3" t="s">
         <v>291</v>
-      </c>
-      <c r="C118" s="3" t="s">
-        <v>292</v>
       </c>
       <c r="D118" s="3" t="s">
         <v>15</v>
@@ -4040,13 +4044,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="119" customHeight="1" ht="18.75">
       <c r="A119" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B119" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="C119" s="3" t="s">
         <v>293</v>
-      </c>
-      <c r="C119" s="3" t="s">
-        <v>294</v>
       </c>
       <c r="D119" s="3" t="s">
         <v>15</v>
@@ -4057,13 +4061,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="120" customHeight="1" ht="18.75">
       <c r="A120" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B120" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="C120" s="3" t="s">
         <v>295</v>
-      </c>
-      <c r="C120" s="3" t="s">
-        <v>296</v>
       </c>
       <c r="D120" s="3" t="s">
         <v>15</v>
@@ -4074,13 +4078,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="121" customHeight="1" ht="18.75">
       <c r="A121" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B121" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="C121" s="3" t="s">
         <v>297</v>
-      </c>
-      <c r="C121" s="3" t="s">
-        <v>298</v>
       </c>
       <c r="D121" s="3" t="s">
         <v>15</v>
@@ -4091,13 +4095,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="122" customHeight="1" ht="18.75">
       <c r="A122" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B122" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="C122" s="3" t="s">
         <v>299</v>
-      </c>
-      <c r="C122" s="3" t="s">
-        <v>300</v>
       </c>
       <c r="D122" s="3" t="s">
         <v>15</v>
@@ -4108,13 +4112,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="123" customHeight="1" ht="18.75">
       <c r="A123" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B123" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="C123" s="3" t="s">
         <v>301</v>
-      </c>
-      <c r="C123" s="3" t="s">
-        <v>302</v>
       </c>
       <c r="D123" s="3" t="s">
         <v>15</v>
@@ -4125,13 +4129,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="124" customHeight="1" ht="18.75">
       <c r="A124" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B124" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="C124" s="3" t="s">
         <v>303</v>
-      </c>
-      <c r="C124" s="3" t="s">
-        <v>304</v>
       </c>
       <c r="D124" s="3" t="s">
         <v>15</v>
@@ -4142,16 +4146,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="125" customHeight="1" ht="18.75">
       <c r="A125" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B125" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="C125" s="3" t="s">
         <v>305</v>
       </c>
-      <c r="C125" s="3" t="s">
-        <v>306</v>
-      </c>
       <c r="D125" s="3" t="s">
-        <v>307</v>
+        <v>15</v>
       </c>
       <c r="E125" s="4">
         <v>1</v>
@@ -4159,16 +4163,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="126" customHeight="1" ht="18.75">
       <c r="A126" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B126" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="C126" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="D126" s="3" t="s">
         <v>308</v>
-      </c>
-      <c r="C126" s="3" t="s">
-        <v>309</v>
-      </c>
-      <c r="D126" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="E126" s="4">
         <v>1</v>
@@ -4176,13 +4180,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="127" customHeight="1" ht="18.75">
       <c r="A127" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B127" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="C127" s="3" t="s">
         <v>310</v>
-      </c>
-      <c r="C127" s="3" t="s">
-        <v>311</v>
       </c>
       <c r="D127" s="3" t="s">
         <v>15</v>
@@ -4193,13 +4197,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="128" customHeight="1" ht="18.75">
       <c r="A128" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B128" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="C128" s="3" t="s">
         <v>312</v>
-      </c>
-      <c r="C128" s="3" t="s">
-        <v>313</v>
       </c>
       <c r="D128" s="3" t="s">
         <v>15</v>
@@ -4210,13 +4214,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="129" customHeight="1" ht="18.75">
       <c r="A129" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B129" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="C129" s="3" t="s">
         <v>314</v>
-      </c>
-      <c r="C129" s="3" t="s">
-        <v>315</v>
       </c>
       <c r="D129" s="3" t="s">
         <v>15</v>
@@ -4227,16 +4231,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="130" customHeight="1" ht="18.75">
       <c r="A130" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B130" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="C130" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="C130" s="3" t="s">
-        <v>317</v>
-      </c>
       <c r="D130" s="3" t="s">
-        <v>318</v>
+        <v>15</v>
       </c>
       <c r="E130" s="4">
         <v>1</v>
@@ -4244,16 +4248,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="131" customHeight="1" ht="18.75">
       <c r="A131" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B131" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="C131" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="D131" s="3" t="s">
         <v>319</v>
-      </c>
-      <c r="C131" s="3" t="s">
-        <v>320</v>
-      </c>
-      <c r="D131" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="E131" s="4">
         <v>1</v>
@@ -4261,13 +4265,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="132" customHeight="1" ht="18.75">
       <c r="A132" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B132" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="C132" s="3" t="s">
         <v>321</v>
-      </c>
-      <c r="C132" s="3" t="s">
-        <v>322</v>
       </c>
       <c r="D132" s="3" t="s">
         <v>15</v>
@@ -4278,16 +4282,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="133" customHeight="1" ht="18.75">
       <c r="A133" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B133" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="C133" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="C133" s="3" t="s">
-        <v>324</v>
-      </c>
       <c r="D133" s="3" t="s">
-        <v>325</v>
+        <v>15</v>
       </c>
       <c r="E133" s="4">
         <v>1</v>
@@ -4295,16 +4299,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="134" customHeight="1" ht="18.75">
       <c r="A134" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B134" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="C134" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="D134" s="3" t="s">
         <v>326</v>
-      </c>
-      <c r="C134" s="3" t="s">
-        <v>327</v>
-      </c>
-      <c r="D134" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="E134" s="4">
         <v>1</v>
@@ -4312,47 +4316,47 @@
     </row>
     <row x14ac:dyDescent="0.25" r="135" customHeight="1" ht="18.75">
       <c r="A135" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B135" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="C135" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="C135" s="3" t="s">
-        <v>329</v>
-      </c>
       <c r="D135" s="3" t="s">
-        <v>330</v>
+        <v>15</v>
       </c>
       <c r="E135" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="136" customHeight="1" ht="18.75">
       <c r="A136" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B136" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="C136" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="D136" s="3" t="s">
         <v>331</v>
       </c>
-      <c r="C136" s="3" t="s">
-        <v>332</v>
-      </c>
-      <c r="D136" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="E136" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="137" customHeight="1" ht="18.75">
       <c r="A137" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B137" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="C137" s="3" t="s">
         <v>333</v>
-      </c>
-      <c r="C137" s="3" t="s">
-        <v>334</v>
       </c>
       <c r="D137" s="3" t="s">
         <v>15</v>
@@ -4363,13 +4367,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="138" customHeight="1" ht="18.75">
       <c r="A138" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B138" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="C138" s="3" t="s">
         <v>335</v>
-      </c>
-      <c r="C138" s="3" t="s">
-        <v>336</v>
       </c>
       <c r="D138" s="3" t="s">
         <v>15</v>
@@ -4380,13 +4384,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="139" customHeight="1" ht="18.75">
       <c r="A139" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B139" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="C139" s="3" t="s">
         <v>337</v>
-      </c>
-      <c r="C139" s="3" t="s">
-        <v>338</v>
       </c>
       <c r="D139" s="3" t="s">
         <v>15</v>
@@ -4397,13 +4401,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="140" customHeight="1" ht="18.75">
       <c r="A140" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B140" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="C140" s="3" t="s">
         <v>339</v>
-      </c>
-      <c r="C140" s="3" t="s">
-        <v>340</v>
       </c>
       <c r="D140" s="3" t="s">
         <v>15</v>
@@ -4414,33 +4418,33 @@
     </row>
     <row x14ac:dyDescent="0.25" r="141" customHeight="1" ht="18.75">
       <c r="A141" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B141" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="C141" s="3" t="s">
         <v>341</v>
       </c>
-      <c r="C141" s="3" t="s">
-        <v>342</v>
-      </c>
       <c r="D141" s="3" t="s">
-        <v>343</v>
+        <v>15</v>
       </c>
       <c r="E141" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="142" customHeight="1" ht="18.75">
       <c r="A142" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B142" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="C142" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="D142" s="3" t="s">
         <v>344</v>
-      </c>
-      <c r="C142" s="3" t="s">
-        <v>345</v>
-      </c>
-      <c r="D142" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="E142" s="4">
         <v>0</v>
@@ -4448,67 +4452,67 @@
     </row>
     <row x14ac:dyDescent="0.25" r="143" customHeight="1" ht="18.75">
       <c r="A143" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B143" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="C143" s="3" t="s">
         <v>346</v>
       </c>
-      <c r="C143" s="3" t="s">
-        <v>347</v>
-      </c>
       <c r="D143" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E143" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="144" customHeight="1" ht="18.75">
       <c r="A144" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B144" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="C144" s="3" t="s">
         <v>348</v>
       </c>
-      <c r="C144" s="3" t="s">
-        <v>349</v>
-      </c>
       <c r="D144" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E144" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="145" customHeight="1" ht="18.75">
       <c r="A145" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B145" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="C145" s="3" t="s">
         <v>350</v>
       </c>
-      <c r="C145" s="3" t="s">
-        <v>351</v>
-      </c>
       <c r="D145" s="3" t="s">
-        <v>352</v>
+        <v>15</v>
       </c>
       <c r="E145" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="146" customHeight="1" ht="18.75">
       <c r="A146" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B146" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="C146" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="D146" s="3" t="s">
         <v>353</v>
-      </c>
-      <c r="C146" s="3" t="s">
-        <v>354</v>
-      </c>
-      <c r="D146" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="E146" s="4">
         <v>1</v>
@@ -4516,13 +4520,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="147" customHeight="1" ht="18.75">
       <c r="A147" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B147" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="C147" s="3" t="s">
         <v>355</v>
-      </c>
-      <c r="C147" s="3" t="s">
-        <v>356</v>
       </c>
       <c r="D147" s="3" t="s">
         <v>15</v>
@@ -4533,13 +4537,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="148" customHeight="1" ht="18.75">
       <c r="A148" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B148" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="C148" s="3" t="s">
         <v>357</v>
-      </c>
-      <c r="C148" s="3" t="s">
-        <v>358</v>
       </c>
       <c r="D148" s="3" t="s">
         <v>15</v>
@@ -4550,33 +4554,33 @@
     </row>
     <row x14ac:dyDescent="0.25" r="149" customHeight="1" ht="18.75">
       <c r="A149" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B149" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="C149" s="3" t="s">
         <v>359</v>
       </c>
-      <c r="C149" s="3" t="s">
-        <v>360</v>
-      </c>
       <c r="D149" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E149" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="150" customHeight="1" ht="18.75">
       <c r="A150" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B150" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="C150" s="3" t="s">
         <v>361</v>
       </c>
-      <c r="C150" s="3" t="s">
-        <v>362</v>
-      </c>
       <c r="D150" s="3" t="s">
-        <v>363</v>
+        <v>15</v>
       </c>
       <c r="E150" s="4">
         <v>0</v>
@@ -4584,16 +4588,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="151" customHeight="1" ht="18.75">
       <c r="A151" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B151" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="C151" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="D151" s="3" t="s">
         <v>364</v>
-      </c>
-      <c r="C151" s="3" t="s">
-        <v>365</v>
-      </c>
-      <c r="D151" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="E151" s="4">
         <v>0</v>
@@ -4601,16 +4605,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="152" customHeight="1" ht="18.75">
       <c r="A152" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B152" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="C152" s="3" t="s">
         <v>366</v>
       </c>
-      <c r="C152" s="3" t="s">
-        <v>367</v>
-      </c>
       <c r="D152" s="3" t="s">
-        <v>368</v>
+        <v>15</v>
       </c>
       <c r="E152" s="4">
         <v>0</v>
@@ -4618,16 +4622,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="153" customHeight="1" ht="18.75">
       <c r="A153" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B153" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="C153" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="D153" s="3" t="s">
         <v>369</v>
-      </c>
-      <c r="C153" s="3" t="s">
-        <v>370</v>
-      </c>
-      <c r="D153" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="E153" s="4">
         <v>0</v>
@@ -4635,16 +4639,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="154" customHeight="1" ht="18.75">
       <c r="A154" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B154" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="C154" s="3" t="s">
         <v>371</v>
       </c>
-      <c r="C154" s="3" t="s">
-        <v>372</v>
-      </c>
       <c r="D154" s="3" t="s">
-        <v>373</v>
+        <v>15</v>
       </c>
       <c r="E154" s="4">
         <v>0</v>
@@ -4652,16 +4656,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="155" customHeight="1" ht="18.75">
       <c r="A155" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B155" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="C155" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="D155" s="3" t="s">
         <v>374</v>
-      </c>
-      <c r="C155" s="3" t="s">
-        <v>375</v>
-      </c>
-      <c r="D155" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="E155" s="4">
         <v>0</v>
@@ -4669,16 +4673,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="156" customHeight="1" ht="18.75">
       <c r="A156" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B156" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="C156" s="3" t="s">
         <v>376</v>
       </c>
-      <c r="C156" s="3" t="s">
-        <v>377</v>
-      </c>
       <c r="D156" s="3" t="s">
-        <v>378</v>
+        <v>15</v>
       </c>
       <c r="E156" s="4">
         <v>0</v>
@@ -4686,16 +4690,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="157" customHeight="1" ht="18.75">
       <c r="A157" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B157" s="3" t="s">
+        <v>377</v>
+      </c>
+      <c r="C157" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="D157" s="3" t="s">
         <v>379</v>
-      </c>
-      <c r="C157" s="3" t="s">
-        <v>380</v>
-      </c>
-      <c r="D157" s="3" t="s">
-        <v>381</v>
       </c>
       <c r="E157" s="4">
         <v>0</v>
@@ -4703,16 +4707,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="158" customHeight="1" ht="18.75">
       <c r="A158" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B158" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="C158" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="D158" s="3" t="s">
         <v>382</v>
-      </c>
-      <c r="C158" s="3" t="s">
-        <v>383</v>
-      </c>
-      <c r="D158" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="E158" s="4">
         <v>0</v>
@@ -4720,50 +4724,50 @@
     </row>
     <row x14ac:dyDescent="0.25" r="159" customHeight="1" ht="18.75">
       <c r="A159" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B159" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="C159" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="C159" s="3" t="s">
-        <v>385</v>
-      </c>
       <c r="D159" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E159" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="160" customHeight="1" ht="18.75">
       <c r="A160" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B160" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="C160" s="3" t="s">
         <v>386</v>
       </c>
-      <c r="C160" s="3" t="s">
-        <v>387</v>
-      </c>
       <c r="D160" s="3" t="s">
-        <v>388</v>
+        <v>15</v>
       </c>
       <c r="E160" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="161" customHeight="1" ht="18.75">
       <c r="A161" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B161" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="C161" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="D161" s="3" t="s">
         <v>389</v>
-      </c>
-      <c r="C161" s="3" t="s">
-        <v>390</v>
-      </c>
-      <c r="D161" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="E161" s="4">
         <v>0</v>
@@ -4771,16 +4775,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="162" customHeight="1" ht="18.75">
       <c r="A162" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B162" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="C162" s="3" t="s">
         <v>391</v>
       </c>
-      <c r="C162" s="3" t="s">
-        <v>392</v>
-      </c>
       <c r="D162" s="3" t="s">
-        <v>393</v>
+        <v>15</v>
       </c>
       <c r="E162" s="4">
         <v>0</v>
@@ -4788,50 +4792,50 @@
     </row>
     <row x14ac:dyDescent="0.25" r="163" customHeight="1" ht="18.75">
       <c r="A163" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="B163" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="C163" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="D163" s="3" t="s">
         <v>394</v>
       </c>
-      <c r="B163" s="3" t="s">
-        <v>395</v>
-      </c>
-      <c r="C163" s="3" t="s">
-        <v>396</v>
-      </c>
-      <c r="D163" s="3" t="s">
-        <v>397</v>
-      </c>
       <c r="E163" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="164" customHeight="1" ht="18.75">
       <c r="A164" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B164" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="C164" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="D164" s="3" t="s">
         <v>398</v>
       </c>
-      <c r="C164" s="3" t="s">
-        <v>399</v>
-      </c>
-      <c r="D164" s="3" t="s">
-        <v>400</v>
-      </c>
       <c r="E164" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="165" customHeight="1" ht="18.75">
       <c r="A165" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B165" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="C165" s="3" t="s">
+        <v>400</v>
+      </c>
+      <c r="D165" s="3" t="s">
         <v>401</v>
-      </c>
-      <c r="C165" s="3" t="s">
-        <v>402</v>
-      </c>
-      <c r="D165" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="E165" s="4">
         <v>0</v>
@@ -4839,13 +4843,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="166" customHeight="1" ht="18.75">
       <c r="A166" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B166" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="C166" s="3" t="s">
         <v>403</v>
-      </c>
-      <c r="C166" s="3" t="s">
-        <v>404</v>
       </c>
       <c r="D166" s="3" t="s">
         <v>15</v>
@@ -4856,47 +4860,47 @@
     </row>
     <row x14ac:dyDescent="0.25" r="167" customHeight="1" ht="18.75">
       <c r="A167" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B167" s="3" t="s">
+        <v>404</v>
+      </c>
+      <c r="C167" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="C167" s="3" t="s">
-        <v>406</v>
-      </c>
       <c r="D167" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E167" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="168" customHeight="1" ht="18.75">
       <c r="A168" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B168" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="C168" s="3" t="s">
         <v>407</v>
       </c>
-      <c r="C168" s="3" t="s">
-        <v>408</v>
-      </c>
       <c r="D168" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E168" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="169" customHeight="1" ht="18.75">
       <c r="A169" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B169" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="C169" s="3" t="s">
         <v>409</v>
-      </c>
-      <c r="C169" s="3" t="s">
-        <v>410</v>
       </c>
       <c r="D169" s="3" t="s">
         <v>15</v>
@@ -4907,13 +4911,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="170" customHeight="1" ht="18.75">
       <c r="A170" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B170" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="C170" s="3" t="s">
         <v>411</v>
-      </c>
-      <c r="C170" s="3" t="s">
-        <v>412</v>
       </c>
       <c r="D170" s="3" t="s">
         <v>15</v>
@@ -4924,33 +4928,33 @@
     </row>
     <row x14ac:dyDescent="0.25" r="171" customHeight="1" ht="18.75">
       <c r="A171" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B171" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="C171" s="3" t="s">
         <v>413</v>
       </c>
-      <c r="C171" s="3" t="s">
-        <v>414</v>
-      </c>
       <c r="D171" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E171" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="172" customHeight="1" ht="18.75">
       <c r="A172" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B172" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="C172" s="3" t="s">
         <v>415</v>
       </c>
-      <c r="C172" s="3" t="s">
-        <v>416</v>
-      </c>
       <c r="D172" s="3" t="s">
-        <v>417</v>
+        <v>15</v>
       </c>
       <c r="E172" s="4">
         <v>1</v>
@@ -4958,33 +4962,33 @@
     </row>
     <row x14ac:dyDescent="0.25" r="173" customHeight="1" ht="18.75">
       <c r="A173" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B173" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="C173" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="D173" s="3" t="s">
         <v>418</v>
       </c>
-      <c r="C173" s="3" t="s">
-        <v>419</v>
-      </c>
-      <c r="D173" s="3" t="s">
-        <v>420</v>
-      </c>
       <c r="E173" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="174" customHeight="1" ht="18.75">
       <c r="A174" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>0</v>
+        <v>419</v>
       </c>
       <c r="C174" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="D174" s="3" t="s">
         <v>421</v>
-      </c>
-      <c r="D174" s="3" t="s">
-        <v>422</v>
       </c>
       <c r="E174" s="4">
         <v>0</v>
@@ -4992,16 +4996,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="175" customHeight="1" ht="18.75">
       <c r="A175" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B175" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C175" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="D175" s="3" t="s">
         <v>423</v>
-      </c>
-      <c r="C175" s="3" t="s">
-        <v>424</v>
-      </c>
-      <c r="D175" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="E175" s="4">
         <v>0</v>
@@ -5009,13 +5013,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="176" customHeight="1" ht="18.75">
       <c r="A176" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B176" s="3" t="s">
+        <v>424</v>
+      </c>
+      <c r="C176" s="3" t="s">
         <v>425</v>
-      </c>
-      <c r="C176" s="3" t="s">
-        <v>426</v>
       </c>
       <c r="D176" s="3" t="s">
         <v>15</v>
@@ -5026,13 +5030,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="177" customHeight="1" ht="18.75">
       <c r="A177" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B177" s="3" t="s">
+        <v>426</v>
+      </c>
+      <c r="C177" s="3" t="s">
         <v>427</v>
-      </c>
-      <c r="C177" s="3" t="s">
-        <v>428</v>
       </c>
       <c r="D177" s="3" t="s">
         <v>15</v>
@@ -5043,16 +5047,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="178" customHeight="1" ht="18.75">
       <c r="A178" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B178" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="C178" s="3" t="s">
         <v>429</v>
       </c>
-      <c r="C178" s="3" t="s">
-        <v>430</v>
-      </c>
       <c r="D178" s="3" t="s">
-        <v>431</v>
+        <v>15</v>
       </c>
       <c r="E178" s="4">
         <v>0</v>
@@ -5060,16 +5064,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="179" customHeight="1" ht="18.75">
       <c r="A179" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B179" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="C179" s="3" t="s">
+        <v>431</v>
+      </c>
+      <c r="D179" s="3" t="s">
         <v>432</v>
-      </c>
-      <c r="C179" s="3" t="s">
-        <v>433</v>
-      </c>
-      <c r="D179" s="3" t="s">
-        <v>434</v>
       </c>
       <c r="E179" s="4">
         <v>0</v>
@@ -5077,16 +5081,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="180" customHeight="1" ht="18.75">
       <c r="A180" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B180" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="C180" s="3" t="s">
+        <v>434</v>
+      </c>
+      <c r="D180" s="3" t="s">
         <v>435</v>
-      </c>
-      <c r="C180" s="3" t="s">
-        <v>436</v>
-      </c>
-      <c r="D180" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="E180" s="4">
         <v>0</v>
@@ -5094,13 +5098,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="181" customHeight="1" ht="18.75">
       <c r="A181" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B181" s="3" t="s">
+        <v>436</v>
+      </c>
+      <c r="C181" s="3" t="s">
         <v>437</v>
-      </c>
-      <c r="C181" s="3" t="s">
-        <v>438</v>
       </c>
       <c r="D181" s="3" t="s">
         <v>15</v>
@@ -5111,16 +5115,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="182" customHeight="1" ht="18.75">
       <c r="A182" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B182" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="C182" s="3" t="s">
         <v>439</v>
       </c>
-      <c r="C182" s="3" t="s">
-        <v>440</v>
-      </c>
       <c r="D182" s="3" t="s">
-        <v>441</v>
+        <v>15</v>
       </c>
       <c r="E182" s="4">
         <v>0</v>
@@ -5128,16 +5132,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="183" customHeight="1" ht="18.75">
       <c r="A183" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B183" s="3" t="s">
+        <v>440</v>
+      </c>
+      <c r="C183" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="D183" s="3" t="s">
         <v>442</v>
-      </c>
-      <c r="C183" s="3" t="s">
-        <v>443</v>
-      </c>
-      <c r="D183" s="3" t="s">
-        <v>444</v>
       </c>
       <c r="E183" s="4">
         <v>0</v>
@@ -5145,16 +5149,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="184" customHeight="1" ht="18.75">
       <c r="A184" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B184" s="3" t="s">
+        <v>443</v>
+      </c>
+      <c r="C184" s="3" t="s">
+        <v>444</v>
+      </c>
+      <c r="D184" s="3" t="s">
         <v>445</v>
-      </c>
-      <c r="C184" s="3" t="s">
-        <v>446</v>
-      </c>
-      <c r="D184" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="E184" s="4">
         <v>0</v>
@@ -5162,13 +5166,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="185" customHeight="1" ht="18.75">
       <c r="A185" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B185" s="3" t="s">
+        <v>446</v>
+      </c>
+      <c r="C185" s="3" t="s">
         <v>447</v>
-      </c>
-      <c r="C185" s="3" t="s">
-        <v>448</v>
       </c>
       <c r="D185" s="3" t="s">
         <v>15</v>
@@ -5179,13 +5183,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="186" customHeight="1" ht="18.75">
       <c r="A186" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B186" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="C186" s="3" t="s">
         <v>449</v>
-      </c>
-      <c r="C186" s="3" t="s">
-        <v>450</v>
       </c>
       <c r="D186" s="3" t="s">
         <v>15</v>
@@ -5196,16 +5200,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="187" customHeight="1" ht="18.75">
       <c r="A187" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B187" s="3" t="s">
+        <v>450</v>
+      </c>
+      <c r="C187" s="3" t="s">
         <v>451</v>
       </c>
-      <c r="C187" s="3" t="s">
-        <v>452</v>
-      </c>
       <c r="D187" s="3" t="s">
-        <v>453</v>
+        <v>15</v>
       </c>
       <c r="E187" s="4">
         <v>0</v>
@@ -5213,16 +5217,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="188" customHeight="1" ht="18.75">
       <c r="A188" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B188" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="C188" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D188" s="3" t="s">
         <v>454</v>
-      </c>
-      <c r="C188" s="3" t="s">
-        <v>455</v>
-      </c>
-      <c r="D188" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="E188" s="4">
         <v>0</v>
@@ -5230,16 +5234,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="189" customHeight="1" ht="18.75">
       <c r="A189" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B189" s="3" t="s">
+        <v>455</v>
+      </c>
+      <c r="C189" s="3" t="s">
         <v>456</v>
       </c>
-      <c r="C189" s="3" t="s">
-        <v>457</v>
-      </c>
       <c r="D189" s="3" t="s">
-        <v>458</v>
+        <v>15</v>
       </c>
       <c r="E189" s="4">
         <v>0</v>
@@ -5247,16 +5251,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="190" customHeight="1" ht="18.75">
       <c r="A190" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B190" s="3" t="s">
+        <v>457</v>
+      </c>
+      <c r="C190" s="3" t="s">
+        <v>458</v>
+      </c>
+      <c r="D190" s="3" t="s">
         <v>459</v>
-      </c>
-      <c r="C190" s="3" t="s">
-        <v>460</v>
-      </c>
-      <c r="D190" s="3" t="s">
-        <v>461</v>
       </c>
       <c r="E190" s="4">
         <v>0</v>
@@ -5264,16 +5268,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="191" customHeight="1" ht="18.75">
       <c r="A191" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B191" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="C191" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="D191" s="3" t="s">
         <v>462</v>
-      </c>
-      <c r="C191" s="3" t="s">
-        <v>463</v>
-      </c>
-      <c r="D191" s="3" t="s">
-        <v>464</v>
       </c>
       <c r="E191" s="4">
         <v>0</v>
@@ -5281,16 +5285,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="192" customHeight="1" ht="18.75">
       <c r="A192" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B192" s="3" t="s">
+        <v>463</v>
+      </c>
+      <c r="C192" s="3" t="s">
+        <v>464</v>
+      </c>
+      <c r="D192" s="3" t="s">
         <v>465</v>
-      </c>
-      <c r="C192" s="3" t="s">
-        <v>466</v>
-      </c>
-      <c r="D192" s="3" t="s">
-        <v>467</v>
       </c>
       <c r="E192" s="4">
         <v>0</v>
@@ -5298,47 +5302,47 @@
     </row>
     <row x14ac:dyDescent="0.25" r="193" customHeight="1" ht="18.75">
       <c r="A193" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B193" s="3" t="s">
+        <v>466</v>
+      </c>
+      <c r="C193" s="3" t="s">
+        <v>467</v>
+      </c>
+      <c r="D193" s="3" t="s">
         <v>468</v>
       </c>
-      <c r="C193" s="3" t="s">
-        <v>469</v>
-      </c>
-      <c r="D193" s="3" t="s">
-        <v>470</v>
-      </c>
       <c r="E193" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="194" customHeight="1" ht="18.75">
       <c r="A194" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B194" s="3" t="s">
+        <v>469</v>
+      </c>
+      <c r="C194" s="3" t="s">
+        <v>470</v>
+      </c>
+      <c r="D194" s="3" t="s">
         <v>471</v>
       </c>
-      <c r="C194" s="3" t="s">
-        <v>472</v>
-      </c>
-      <c r="D194" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="E194" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="195" customHeight="1" ht="18.75">
       <c r="A195" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B195" s="3" t="s">
+        <v>472</v>
+      </c>
+      <c r="C195" s="3" t="s">
         <v>473</v>
-      </c>
-      <c r="C195" s="3" t="s">
-        <v>474</v>
       </c>
       <c r="D195" s="3" t="s">
         <v>15</v>
@@ -5349,13 +5353,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="196" customHeight="1" ht="18.75">
       <c r="A196" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B196" s="3" t="s">
+        <v>474</v>
+      </c>
+      <c r="C196" s="3" t="s">
         <v>475</v>
-      </c>
-      <c r="C196" s="3" t="s">
-        <v>476</v>
       </c>
       <c r="D196" s="3" t="s">
         <v>15</v>
@@ -5366,13 +5370,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="197" customHeight="1" ht="18.75">
       <c r="A197" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B197" s="3" t="s">
+        <v>476</v>
+      </c>
+      <c r="C197" s="3" t="s">
         <v>477</v>
-      </c>
-      <c r="C197" s="3" t="s">
-        <v>478</v>
       </c>
       <c r="D197" s="3" t="s">
         <v>15</v>
@@ -5383,13 +5387,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="198" customHeight="1" ht="18.75">
       <c r="A198" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B198" s="3" t="s">
+        <v>478</v>
+      </c>
+      <c r="C198" s="3" t="s">
         <v>479</v>
-      </c>
-      <c r="C198" s="3" t="s">
-        <v>480</v>
       </c>
       <c r="D198" s="3" t="s">
         <v>15</v>
@@ -5400,13 +5404,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="199" customHeight="1" ht="18.75">
       <c r="A199" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B199" s="3" t="s">
+        <v>480</v>
+      </c>
+      <c r="C199" s="3" t="s">
         <v>481</v>
-      </c>
-      <c r="C199" s="3" t="s">
-        <v>482</v>
       </c>
       <c r="D199" s="3" t="s">
         <v>15</v>
@@ -5417,13 +5421,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="200" customHeight="1" ht="18.75">
       <c r="A200" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B200" s="3" t="s">
+        <v>482</v>
+      </c>
+      <c r="C200" s="3" t="s">
         <v>483</v>
-      </c>
-      <c r="C200" s="3" t="s">
-        <v>484</v>
       </c>
       <c r="D200" s="3" t="s">
         <v>15</v>
@@ -5434,13 +5438,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="201" customHeight="1" ht="18.75">
       <c r="A201" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B201" s="3" t="s">
+        <v>484</v>
+      </c>
+      <c r="C201" s="3" t="s">
         <v>485</v>
-      </c>
-      <c r="C201" s="3" t="s">
-        <v>486</v>
       </c>
       <c r="D201" s="3" t="s">
         <v>15</v>
@@ -5451,13 +5455,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="202" customHeight="1" ht="18.75">
       <c r="A202" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B202" s="3" t="s">
+        <v>486</v>
+      </c>
+      <c r="C202" s="3" t="s">
         <v>487</v>
-      </c>
-      <c r="C202" s="3" t="s">
-        <v>488</v>
       </c>
       <c r="D202" s="3" t="s">
         <v>15</v>
@@ -5468,13 +5472,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="203" customHeight="1" ht="18.75">
       <c r="A203" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B203" s="3" t="s">
+        <v>488</v>
+      </c>
+      <c r="C203" s="3" t="s">
         <v>489</v>
-      </c>
-      <c r="C203" s="3" t="s">
-        <v>490</v>
       </c>
       <c r="D203" s="3" t="s">
         <v>15</v>
@@ -5485,13 +5489,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="204" customHeight="1" ht="18.75">
       <c r="A204" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B204" s="3" t="s">
+        <v>490</v>
+      </c>
+      <c r="C204" s="3" t="s">
         <v>491</v>
-      </c>
-      <c r="C204" s="3" t="s">
-        <v>492</v>
       </c>
       <c r="D204" s="3" t="s">
         <v>15</v>
@@ -5502,13 +5506,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="205" customHeight="1" ht="18.75">
       <c r="A205" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B205" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="C205" s="3" t="s">
         <v>493</v>
-      </c>
-      <c r="C205" s="3" t="s">
-        <v>494</v>
       </c>
       <c r="D205" s="3" t="s">
         <v>15</v>
@@ -5519,13 +5523,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="206" customHeight="1" ht="18.75">
       <c r="A206" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B206" s="3" t="s">
+        <v>494</v>
+      </c>
+      <c r="C206" s="3" t="s">
         <v>495</v>
-      </c>
-      <c r="C206" s="3" t="s">
-        <v>496</v>
       </c>
       <c r="D206" s="3" t="s">
         <v>15</v>
@@ -5536,13 +5540,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="207" customHeight="1" ht="18.75">
       <c r="A207" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B207" s="3" t="s">
+        <v>496</v>
+      </c>
+      <c r="C207" s="3" t="s">
         <v>497</v>
-      </c>
-      <c r="C207" s="3" t="s">
-        <v>498</v>
       </c>
       <c r="D207" s="3" t="s">
         <v>15</v>
@@ -5553,13 +5557,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="208" customHeight="1" ht="18.75">
       <c r="A208" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B208" s="3" t="s">
+        <v>498</v>
+      </c>
+      <c r="C208" s="3" t="s">
         <v>499</v>
-      </c>
-      <c r="C208" s="3" t="s">
-        <v>500</v>
       </c>
       <c r="D208" s="3" t="s">
         <v>15</v>
@@ -5570,13 +5574,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="209" customHeight="1" ht="18.75">
       <c r="A209" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B209" s="3" t="s">
+        <v>500</v>
+      </c>
+      <c r="C209" s="3" t="s">
         <v>501</v>
-      </c>
-      <c r="C209" s="3" t="s">
-        <v>502</v>
       </c>
       <c r="D209" s="3" t="s">
         <v>15</v>
@@ -5587,13 +5591,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="210" customHeight="1" ht="18.75">
       <c r="A210" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B210" s="3" t="s">
+        <v>502</v>
+      </c>
+      <c r="C210" s="3" t="s">
         <v>503</v>
-      </c>
-      <c r="C210" s="3" t="s">
-        <v>504</v>
       </c>
       <c r="D210" s="3" t="s">
         <v>15</v>
@@ -5604,13 +5608,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="211" customHeight="1" ht="18.75">
       <c r="A211" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B211" s="3" t="s">
+        <v>504</v>
+      </c>
+      <c r="C211" s="3" t="s">
         <v>505</v>
-      </c>
-      <c r="C211" s="3" t="s">
-        <v>506</v>
       </c>
       <c r="D211" s="3" t="s">
         <v>15</v>
@@ -5621,13 +5625,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="212" customHeight="1" ht="18.75">
       <c r="A212" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B212" s="3" t="s">
+        <v>506</v>
+      </c>
+      <c r="C212" s="3" t="s">
         <v>507</v>
-      </c>
-      <c r="C212" s="3" t="s">
-        <v>508</v>
       </c>
       <c r="D212" s="3" t="s">
         <v>15</v>
@@ -5638,13 +5642,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="213" customHeight="1" ht="18.75">
       <c r="A213" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B213" s="3" t="s">
+        <v>508</v>
+      </c>
+      <c r="C213" s="3" t="s">
         <v>509</v>
-      </c>
-      <c r="C213" s="3" t="s">
-        <v>510</v>
       </c>
       <c r="D213" s="3" t="s">
         <v>15</v>
@@ -5655,13 +5659,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="214" customHeight="1" ht="18.75">
       <c r="A214" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B214" s="3" t="s">
+        <v>510</v>
+      </c>
+      <c r="C214" s="3" t="s">
         <v>511</v>
-      </c>
-      <c r="C214" s="3" t="s">
-        <v>512</v>
       </c>
       <c r="D214" s="3" t="s">
         <v>15</v>
@@ -5672,13 +5676,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="215" customHeight="1" ht="18.75">
       <c r="A215" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B215" s="3" t="s">
+        <v>512</v>
+      </c>
+      <c r="C215" s="3" t="s">
         <v>513</v>
-      </c>
-      <c r="C215" s="3" t="s">
-        <v>514</v>
       </c>
       <c r="D215" s="3" t="s">
         <v>15</v>
@@ -5689,13 +5693,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="216" customHeight="1" ht="18.75">
       <c r="A216" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B216" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="C216" s="3" t="s">
         <v>515</v>
-      </c>
-      <c r="C216" s="3" t="s">
-        <v>516</v>
       </c>
       <c r="D216" s="3" t="s">
         <v>15</v>
@@ -5706,13 +5710,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="217" customHeight="1" ht="18.75">
       <c r="A217" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B217" s="3" t="s">
+        <v>516</v>
+      </c>
+      <c r="C217" s="3" t="s">
         <v>517</v>
-      </c>
-      <c r="C217" s="3" t="s">
-        <v>518</v>
       </c>
       <c r="D217" s="3" t="s">
         <v>15</v>
@@ -5723,13 +5727,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="218" customHeight="1" ht="18.75">
       <c r="A218" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B218" s="3" t="s">
+        <v>518</v>
+      </c>
+      <c r="C218" s="3" t="s">
         <v>519</v>
-      </c>
-      <c r="C218" s="3" t="s">
-        <v>520</v>
       </c>
       <c r="D218" s="3" t="s">
         <v>15</v>
@@ -5740,13 +5744,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="219" customHeight="1" ht="18.75">
       <c r="A219" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B219" s="3" t="s">
+        <v>520</v>
+      </c>
+      <c r="C219" s="3" t="s">
         <v>521</v>
-      </c>
-      <c r="C219" s="3" t="s">
-        <v>522</v>
       </c>
       <c r="D219" s="3" t="s">
         <v>15</v>
@@ -5757,13 +5761,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="220" customHeight="1" ht="18.75">
       <c r="A220" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B220" s="3" t="s">
+        <v>522</v>
+      </c>
+      <c r="C220" s="3" t="s">
         <v>523</v>
-      </c>
-      <c r="C220" s="3" t="s">
-        <v>524</v>
       </c>
       <c r="D220" s="3" t="s">
         <v>15</v>
@@ -5774,13 +5778,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="221" customHeight="1" ht="18.75">
       <c r="A221" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B221" s="3" t="s">
+        <v>524</v>
+      </c>
+      <c r="C221" s="3" t="s">
         <v>525</v>
-      </c>
-      <c r="C221" s="3" t="s">
-        <v>526</v>
       </c>
       <c r="D221" s="3" t="s">
         <v>15</v>
@@ -5791,13 +5795,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="222" customHeight="1" ht="18.75">
       <c r="A222" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B222" s="3" t="s">
+        <v>526</v>
+      </c>
+      <c r="C222" s="3" t="s">
         <v>527</v>
-      </c>
-      <c r="C222" s="3" t="s">
-        <v>528</v>
       </c>
       <c r="D222" s="3" t="s">
         <v>15</v>
@@ -5808,13 +5812,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="223" customHeight="1" ht="18.75">
       <c r="A223" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B223" s="3" t="s">
+        <v>528</v>
+      </c>
+      <c r="C223" s="3" t="s">
         <v>529</v>
-      </c>
-      <c r="C223" s="3" t="s">
-        <v>530</v>
       </c>
       <c r="D223" s="3" t="s">
         <v>15</v>
@@ -5825,16 +5829,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="224" customHeight="1" ht="18.75">
       <c r="A224" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B224" s="3" t="s">
+        <v>530</v>
+      </c>
+      <c r="C224" s="3" t="s">
         <v>531</v>
       </c>
-      <c r="C224" s="3" t="s">
-        <v>532</v>
-      </c>
       <c r="D224" s="3" t="s">
-        <v>533</v>
+        <v>15</v>
       </c>
       <c r="E224" s="4">
         <v>0</v>
@@ -5842,16 +5846,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="225" customHeight="1" ht="18.75">
       <c r="A225" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B225" s="3" t="s">
+        <v>532</v>
+      </c>
+      <c r="C225" s="3" t="s">
+        <v>533</v>
+      </c>
+      <c r="D225" s="3" t="s">
         <v>534</v>
-      </c>
-      <c r="C225" s="3" t="s">
-        <v>535</v>
-      </c>
-      <c r="D225" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="E225" s="4">
         <v>0</v>
@@ -5859,20 +5863,24 @@
     </row>
     <row x14ac:dyDescent="0.25" r="226" customHeight="1" ht="18.75">
       <c r="A226" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B226" s="3" t="s">
+        <v>535</v>
+      </c>
+      <c r="C226" s="3" t="s">
         <v>536</v>
       </c>
-      <c r="C226" s="3"/>
-      <c r="D226" s="3"/>
+      <c r="D226" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="E226" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="227" customHeight="1" ht="18.75">
       <c r="A227" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B227" s="3" t="s">
         <v>537</v>
@@ -5885,7 +5893,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="228" customHeight="1" ht="18.75">
       <c r="A228" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B228" s="3" t="s">
         <v>538</v>
@@ -5898,7 +5906,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="229" customHeight="1" ht="18.75">
       <c r="A229" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B229" s="3" t="s">
         <v>539</v>
@@ -5911,7 +5919,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="230" customHeight="1" ht="18.75">
       <c r="A230" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B230" s="3" t="s">
         <v>540</v>
@@ -5924,7 +5932,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="231" customHeight="1" ht="18.75">
       <c r="A231" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B231" s="3" t="s">
         <v>541</v>
@@ -5937,7 +5945,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="232" customHeight="1" ht="18.75">
       <c r="A232" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B232" s="3" t="s">
         <v>542</v>
@@ -5950,7 +5958,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="233" customHeight="1" ht="18.75">
       <c r="A233" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B233" s="3" t="s">
         <v>543</v>
@@ -5961,9 +5969,9 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="234" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="234" customHeight="1" ht="18.75">
       <c r="A234" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B234" s="3" t="s">
         <v>544</v>
@@ -5971,6 +5979,19 @@
       <c r="C234" s="3"/>
       <c r="D234" s="3"/>
       <c r="E234" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="235" customHeight="1" ht="19.5">
+      <c r="A235" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="B235" s="3" t="s">
+        <v>545</v>
+      </c>
+      <c r="C235" s="3"/>
+      <c r="D235" s="3"/>
+      <c r="E235" s="4">
         <v>1</v>
       </c>
     </row>

</xml_diff>